<commit_message>
Fix H2 row and if column in matriz_sintaxis file
</commit_message>
<xml_diff>
--- a/src/resources/matriz_sintaxis.xlsx
+++ b/src/resources/matriz_sintaxis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguir\Desktop\compi\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810343E4-3BF3-4F87-A707-8C8AD2AC2B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C6326F-95E5-4EC9-A2AD-3CEAB25E8769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{D6C56674-CF05-41A6-99FF-8D906A4082A8}"/>
   </bookViews>
@@ -1205,9 +1205,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4674143A-35AC-4966-BCD5-4F09074A1FC3}">
   <dimension ref="A1:EA201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AO33" sqref="AO33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13917,8 +13917,8 @@
       <c r="C33" s="8">
         <v>527</v>
       </c>
-      <c r="D33" s="8">
-        <v>527</v>
+      <c r="D33" s="10">
+        <v>66</v>
       </c>
       <c r="E33" s="9">
         <v>184</v>
@@ -13926,8 +13926,8 @@
       <c r="F33" s="8">
         <v>527</v>
       </c>
-      <c r="G33" s="8">
-        <v>527</v>
+      <c r="G33" s="10">
+        <v>66</v>
       </c>
       <c r="H33" s="8">
         <v>527</v>
@@ -13944,14 +13944,14 @@
       <c r="L33" s="9">
         <v>184</v>
       </c>
-      <c r="M33" s="8">
-        <v>527</v>
+      <c r="M33" s="10">
+        <v>66</v>
       </c>
       <c r="N33" s="9">
         <v>184</v>
       </c>
-      <c r="O33" s="8">
-        <v>527</v>
+      <c r="O33" s="10">
+        <v>66</v>
       </c>
       <c r="P33" s="9">
         <v>184</v>
@@ -13971,14 +13971,14 @@
       <c r="U33" s="9">
         <v>184</v>
       </c>
-      <c r="V33" s="8">
-        <v>527</v>
+      <c r="V33" s="10">
+        <v>66</v>
       </c>
       <c r="W33" s="9">
         <v>184</v>
       </c>
-      <c r="X33" s="8">
-        <v>527</v>
+      <c r="X33" s="10">
+        <v>66</v>
       </c>
       <c r="Y33" s="8">
         <v>527</v>
@@ -13986,8 +13986,8 @@
       <c r="Z33" s="9">
         <v>184</v>
       </c>
-      <c r="AA33" s="8">
-        <v>527</v>
+      <c r="AA33" s="10">
+        <v>66</v>
       </c>
       <c r="AB33" s="9">
         <v>184</v>
@@ -14001,8 +14001,8 @@
       <c r="AE33" s="9">
         <v>184</v>
       </c>
-      <c r="AF33" s="8">
-        <v>527</v>
+      <c r="AF33" s="10">
+        <v>66</v>
       </c>
       <c r="AG33" s="9">
         <v>184</v>
@@ -14013,17 +14013,17 @@
       <c r="AI33" s="9">
         <v>184</v>
       </c>
-      <c r="AJ33" s="8">
-        <v>527</v>
+      <c r="AJ33" s="10">
+        <v>66</v>
       </c>
       <c r="AK33" s="9">
         <v>184</v>
       </c>
-      <c r="AL33" s="8">
-        <v>527</v>
-      </c>
-      <c r="AM33" s="8">
-        <v>527</v>
+      <c r="AL33" s="10">
+        <v>66</v>
+      </c>
+      <c r="AM33" s="10">
+        <v>66</v>
       </c>
       <c r="AN33" s="8">
         <v>527</v>
@@ -24364,8 +24364,8 @@
       <c r="BJ59" s="8">
         <v>542</v>
       </c>
-      <c r="BK59" s="8">
-        <v>542</v>
+      <c r="BK59" s="10">
+        <v>132</v>
       </c>
       <c r="BL59" s="8">
         <v>542</v>
@@ -25154,8 +25154,8 @@
       <c r="BJ61" s="8">
         <v>543</v>
       </c>
-      <c r="BK61" s="8">
-        <v>543</v>
+      <c r="BK61" s="10">
+        <v>135</v>
       </c>
       <c r="BL61" s="8">
         <v>543</v>
@@ -35029,8 +35029,8 @@
       <c r="BJ86" s="8">
         <v>554</v>
       </c>
-      <c r="BK86" s="8">
-        <v>554</v>
+      <c r="BK86" s="10">
+        <v>178</v>
       </c>
       <c r="BL86" s="8">
         <v>554</v>
@@ -35819,8 +35819,8 @@
       <c r="BJ88" s="8">
         <v>555</v>
       </c>
-      <c r="BK88" s="8">
-        <v>555</v>
+      <c r="BK88" s="10">
+        <v>181</v>
       </c>
       <c r="BL88" s="8">
         <v>555</v>

</xml_diff>